<commit_message>
add data for 01-14-2021
</commit_message>
<xml_diff>
--- a/StockWatchListJan2021.xlsx
+++ b/StockWatchListJan2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahk\Desktop\Project\StockRecords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1BB4F71-4A2A-42D2-B3E3-C5007C8B7CFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31A5907-F4F6-4343-B5AF-74D7D1C9B11D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="5" xr2:uid="{651882B6-81FE-4D1C-AFC3-A83B7F4B66C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="6" xr2:uid="{651882B6-81FE-4D1C-AFC3-A83B7F4B66C8}"/>
   </bookViews>
   <sheets>
     <sheet name="2021-01-04" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="2021-01-11" sheetId="8" r:id="rId4"/>
     <sheet name="2021-01-12" sheetId="9" r:id="rId5"/>
     <sheet name="2021-01-13" sheetId="10" r:id="rId6"/>
+    <sheet name="2021-01-14" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="53">
   <si>
     <t>Raytheon Technologies Corporation (RTX)</t>
   </si>
@@ -218,6 +219,21 @@
   </si>
   <si>
     <t>Walmart Inc. (WMT)</t>
+  </si>
+  <si>
+    <t>JPMorgan Chase &amp;amp; Co. (JPM)</t>
+  </si>
+  <si>
+    <t>BEST Inc. (BEST)</t>
+  </si>
+  <si>
+    <t>Minerals Technologies Inc. (MTX)</t>
+  </si>
+  <si>
+    <t>Cresco Labs Inc. (CRLBF)</t>
+  </si>
+  <si>
+    <t>volume</t>
   </si>
 </sst>
 </file>
@@ -376,7 +392,15 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="42">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -397,6 +421,20 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -516,17 +554,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12100C39-EE12-41D9-AB51-17C1D8610CFA}" name="Table3" displayName="Table3" ref="A1:F24" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12100C39-EE12-41D9-AB51-17C1D8610CFA}" name="Table3" displayName="Table3" ref="A1:F24" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:F24" xr:uid="{6EF38450-56CB-4C63-B38D-E59685B2599D}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6FD60834-A872-42A1-A8DC-830168D15993}" name="Stock" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{6FD60834-A872-42A1-A8DC-830168D15993}" name="Stock" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{46A0D2B8-37D4-4E2D-BDEA-9D6DA32FCC5C}" name="Current"/>
-    <tableColumn id="3" xr3:uid="{E9C355AD-35E4-43A4-A7FC-E3C26445E593}" name="Low" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{22E09959-9B7B-4C83-8609-48C4B14D681E}" name="High" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{F67D3D68-38E8-4A7E-8DFD-7FC255DC5AB4}" name="Current vs Low" dataDxfId="30">
+    <tableColumn id="3" xr3:uid="{E9C355AD-35E4-43A4-A7FC-E3C26445E593}" name="Low" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{22E09959-9B7B-4C83-8609-48C4B14D681E}" name="High" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{F67D3D68-38E8-4A7E-8DFD-7FC255DC5AB4}" name="Current vs Low" dataDxfId="36">
       <calculatedColumnFormula>($B2-$C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2F24A522-54F7-4841-ACDA-118F051C8FCE}" name="Current vs High" dataDxfId="29">
+    <tableColumn id="6" xr3:uid="{2F24A522-54F7-4841-ACDA-118F051C8FCE}" name="Current vs High" dataDxfId="35">
       <calculatedColumnFormula>($B2-$D2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -535,20 +573,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{81F2F2C0-2C9F-407F-99CA-7ED7FF00BC4A}" name="Table36" displayName="Table36" ref="A1:G25" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{81F2F2C0-2C9F-407F-99CA-7ED7FF00BC4A}" name="Table36" displayName="Table36" ref="A1:G25" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A1:G25" xr:uid="{6EF38450-56CB-4C63-B38D-E59685B2599D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BFBE3B85-C0CE-4D48-86E2-E25EDB75289A}" name="Stock" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{BFBE3B85-C0CE-4D48-86E2-E25EDB75289A}" name="Stock" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{7EFA2E9E-6285-4FBB-8DBE-01FC9DD451E9}" name="Current"/>
     <tableColumn id="3" xr3:uid="{6CE43BF0-02E7-44FE-8AC8-EFFA6BDDDF94}" name="Low"/>
     <tableColumn id="4" xr3:uid="{9600C03C-8E5D-4624-926C-6499F5D908DF}" name="High"/>
-    <tableColumn id="5" xr3:uid="{5A5854C7-6028-4851-85D1-909A07C06307}" name="Current vs Low" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{5A5854C7-6028-4851-85D1-909A07C06307}" name="Current vs Low" dataDxfId="31">
       <calculatedColumnFormula>($B2-$C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{331EBF5D-1B2D-4479-A71A-2222C8749ED9}" name="Current vs High" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{331EBF5D-1B2D-4479-A71A-2222C8749ED9}" name="Current vs High" dataDxfId="30">
       <calculatedColumnFormula>($B2-$D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1814E88C-57E3-42CA-9026-4A1D6B3412FF}" name="From Start" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{1814E88C-57E3-42CA-9026-4A1D6B3412FF}" name="From Start" dataDxfId="29">
       <calculatedColumnFormula>(B2-'2021-01-04'!$B2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -557,20 +595,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C115F6F-F687-48A3-96D9-E248C31F9A97}" name="Table362" displayName="Table362" ref="A1:G29" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C115F6F-F687-48A3-96D9-E248C31F9A97}" name="Table362" displayName="Table362" ref="A1:G29" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:G29" xr:uid="{6EF38450-56CB-4C63-B38D-E59685B2599D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F8D643F5-192D-4766-906C-27C88FDFBF83}" name="Stock" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{F8D643F5-192D-4766-906C-27C88FDFBF83}" name="Stock" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{F4EBA0D4-DDD0-4411-A46B-5FB8E43AA419}" name="Current"/>
     <tableColumn id="3" xr3:uid="{281CFC7B-D1D7-4578-AB00-4A96B0CE2A5A}" name="Low"/>
     <tableColumn id="4" xr3:uid="{D7495BAF-B505-42F9-A9CB-4D80A0C46276}" name="High"/>
-    <tableColumn id="5" xr3:uid="{4CD64326-9876-461E-B097-B6108C0F6593}" name="Current vs Low" dataDxfId="19">
+    <tableColumn id="5" xr3:uid="{4CD64326-9876-461E-B097-B6108C0F6593}" name="Current vs Low" dataDxfId="25">
       <calculatedColumnFormula>($B2-$C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{94D8CF8F-24FC-49CA-8A5D-5F33D21F34E7}" name="Current vs High" dataDxfId="18">
+    <tableColumn id="6" xr3:uid="{94D8CF8F-24FC-49CA-8A5D-5F33D21F34E7}" name="Current vs High" dataDxfId="24">
       <calculatedColumnFormula>($B2-$D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7537865B-A6A5-4A32-937B-9091C2673D70}" name="From Start" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{7537865B-A6A5-4A32-937B-9091C2673D70}" name="From Start" dataDxfId="23">
       <calculatedColumnFormula>(B2-'2021-01-05'!$B2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -579,20 +617,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9D160409-900E-4C16-9B85-3467A6536478}" name="Table3625" displayName="Table3625" ref="A1:G31" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9D160409-900E-4C16-9B85-3467A6536478}" name="Table3625" displayName="Table3625" ref="A1:G31" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:G31" xr:uid="{6EF38450-56CB-4C63-B38D-E59685B2599D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0D44B704-F135-4180-AA82-8FCF9CC99181}" name="Stock" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{0D44B704-F135-4180-AA82-8FCF9CC99181}" name="Stock" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{B089DF6F-4CA4-4B4B-A9FD-92100E95A646}" name="Current"/>
     <tableColumn id="3" xr3:uid="{C134F852-91AF-497F-9A8F-8CA48DA8F03E}" name="Low"/>
     <tableColumn id="4" xr3:uid="{58AB1DC9-2FA1-4611-B208-FCB49BA7815E}" name="High"/>
-    <tableColumn id="5" xr3:uid="{98C23A6F-3439-47BF-975F-D1D298242A1A}" name="Current vs Low" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{98C23A6F-3439-47BF-975F-D1D298242A1A}" name="Current vs Low" dataDxfId="19">
       <calculatedColumnFormula>($B2-$C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{80084716-F5C8-4703-BA67-F0B740142295}" name="Current vs High" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{80084716-F5C8-4703-BA67-F0B740142295}" name="Current vs High" dataDxfId="18">
       <calculatedColumnFormula>($B2-$D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D594E6E0-BF0B-470B-8E76-30C24001FE92}" name="From Start" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{D594E6E0-BF0B-470B-8E76-30C24001FE92}" name="From Start" dataDxfId="17">
       <calculatedColumnFormula>(B2-'2021-01-07'!$B2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -601,20 +639,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CA6AF04A-370D-46CC-AC33-CF0B3584784C}" name="Table36253" displayName="Table36253" ref="A1:G32" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CA6AF04A-370D-46CC-AC33-CF0B3584784C}" name="Table36253" displayName="Table36253" ref="A1:G32" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:G32" xr:uid="{6EF38450-56CB-4C63-B38D-E59685B2599D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2CD234DF-61E3-4DA7-97AE-2279DC9AAA5D}" name="Stock" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{2CD234DF-61E3-4DA7-97AE-2279DC9AAA5D}" name="Stock" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{2A513CD4-2B43-4FAD-ABA4-1931C7549442}" name="Current"/>
     <tableColumn id="3" xr3:uid="{AD8A1F44-9CA9-45BC-A2A3-64A89B0FFEA8}" name="Low"/>
     <tableColumn id="4" xr3:uid="{F7785626-26F9-408C-B8CF-2BEEE10F58EF}" name="High"/>
-    <tableColumn id="5" xr3:uid="{3452AD13-DDC6-45E1-B0B8-53D1621A68AE}" name="Current vs Low" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{3452AD13-DDC6-45E1-B0B8-53D1621A68AE}" name="Current vs Low" dataDxfId="13">
       <calculatedColumnFormula>($B2-$C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{10910D0E-A528-4CE0-ACE9-BC61E83DF25B}" name="Current vs High" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{10910D0E-A528-4CE0-ACE9-BC61E83DF25B}" name="Current vs High" dataDxfId="12">
       <calculatedColumnFormula>($B2-$D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{106ADCB7-6A38-45D7-AD5E-C978E26F5BE6}" name="From Start" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{106ADCB7-6A38-45D7-AD5E-C978E26F5BE6}" name="From Start" dataDxfId="1">
       <calculatedColumnFormula>(B2-'2021-01-11'!$B2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -623,20 +661,43 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EFE2B2B9-1FF6-49D3-81AE-D806A8CA4455}" name="Table362537" displayName="Table362537" ref="A1:G37" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EFE2B2B9-1FF6-49D3-81AE-D806A8CA4455}" name="Table362537" displayName="Table362537" ref="A1:G37" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:G37" xr:uid="{6EF38450-56CB-4C63-B38D-E59685B2599D}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D48366B4-7049-4EAC-88D7-0ECF2F4A10A3}" name="Stock"/>
     <tableColumn id="2" xr3:uid="{9813A389-01CC-4057-B9A7-98AC4EFF4206}" name="Current"/>
     <tableColumn id="3" xr3:uid="{DC73F1C2-63F5-4A09-B923-3BA9FB95F0A9}" name="Low"/>
     <tableColumn id="4" xr3:uid="{5BD95DD2-F8F5-42F3-A560-FF7CE57C0D30}" name="High"/>
-    <tableColumn id="5" xr3:uid="{07EB3F6C-05E0-4C4E-8BD8-AD46CCF5CFEA}" name="Current vs Low" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{07EB3F6C-05E0-4C4E-8BD8-AD46CCF5CFEA}" name="Current vs Low" dataDxfId="9">
       <calculatedColumnFormula>($B2-$C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{ABFE05F1-3D31-470D-A8B9-250DE086D37F}" name="Current vs High" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{ABFE05F1-3D31-470D-A8B9-250DE086D37F}" name="Current vs High" dataDxfId="8">
       <calculatedColumnFormula>($B2-$D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{22431159-8E37-4D72-BE17-936CC4CDD256}" name="From Start" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{22431159-8E37-4D72-BE17-936CC4CDD256}" name="From Start" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F32F30F2-3EEC-42D8-B2A2-441556119865}" name="Table3625378" displayName="Table3625378" ref="A1:H41" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:H41" xr:uid="{6EF38450-56CB-4C63-B38D-E59685B2599D}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{CEE43F61-84D4-4AE6-B6D0-768E15A41598}" name="Stock"/>
+    <tableColumn id="2" xr3:uid="{C302D760-E0DC-4A16-A2C7-B0119B32F2E9}" name="Current"/>
+    <tableColumn id="3" xr3:uid="{D67CC75A-C315-4796-8492-388CA0380907}" name="Low"/>
+    <tableColumn id="4" xr3:uid="{350FAA28-0A55-4C5E-BC96-ED84818C1324}" name="High"/>
+    <tableColumn id="5" xr3:uid="{06FE4CAA-23DF-4ED1-8557-40F56958C9E6}" name="Current vs Low" dataDxfId="4">
+      <calculatedColumnFormula>($B2-$C2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{89E9CDC0-31FA-47CB-AF7C-5841FB6EAC24}" name="Current vs High" dataDxfId="3">
+      <calculatedColumnFormula>($B2-$D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{1C8FAD60-1F61-44EC-A4D5-14796DD6726D}" name="From Start" dataDxfId="0">
+      <calculatedColumnFormula>(B2-'2021-01-13'!$B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{3772E1EF-9D3F-42EE-B5D3-605BA6068B3D}" name="volume" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3780,7 +3841,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4632,7 +4693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AE4536-25C6-4139-99D2-1B87E135C911}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
@@ -5500,4 +5561,1214 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CC7F5E-704B-4B62-8EEC-4F356281C61F}">
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="4" width="11" customWidth="1"/>
+    <col min="5" max="6" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>128.83000000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>126.48</v>
+      </c>
+      <c r="D2" s="1">
+        <v>132.56</v>
+      </c>
+      <c r="E2" s="1">
+        <f>($B2-$C2)</f>
+        <v>2.3500000000000085</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F24" si="0">($B2-$D2)</f>
+        <v>-3.7299999999999898</v>
+      </c>
+      <c r="G2" s="6">
+        <f>(B2-'2021-01-13'!$B2)</f>
+        <v>-2.0599999999999739</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5120744</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>23.66</v>
+      </c>
+      <c r="C3" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>24.84</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E23" si="1">($B3-$C3)</f>
+        <v>0.46000000000000085</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.1799999999999997</v>
+      </c>
+      <c r="G3">
+        <f>(B3-'2021-01-13'!$B3)</f>
+        <v>8.0000000000001847E-2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>13507827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40.22</v>
+      </c>
+      <c r="C4" s="1">
+        <v>37.24</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40.22</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9799999999999969</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <f>(B4-'2021-01-13'!$B4)</f>
+        <v>1.9799999999999969</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1760252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>36.19</v>
+      </c>
+      <c r="C5" s="1">
+        <v>34.6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5899999999999963</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.81000000000000227</v>
+      </c>
+      <c r="G5" s="1">
+        <f>(B5-'2021-01-13'!$B5)</f>
+        <v>0.14000000000000057</v>
+      </c>
+      <c r="H5" s="2">
+        <v>7341514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>220.43</v>
+      </c>
+      <c r="C6" s="1">
+        <v>200.89</v>
+      </c>
+      <c r="D6" s="1">
+        <v>227.03</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>19.54000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.5999999999999943</v>
+      </c>
+      <c r="G6" s="6">
+        <f>(B6-'2021-01-13'!$B6)</f>
+        <v>-3.3299999999999841</v>
+      </c>
+      <c r="H6" s="2">
+        <v>776287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="C7" s="1">
+        <v>17.36</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20.75</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9699999999999989</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.42000000000000171</v>
+      </c>
+      <c r="G7" s="1">
+        <f>(B7-'2021-01-13'!$B7)</f>
+        <v>1.1999999999999993</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10443903</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>23.76</v>
+      </c>
+      <c r="C8" s="1">
+        <v>21.37</v>
+      </c>
+      <c r="D8" s="1">
+        <v>25.57</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3900000000000006</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.8099999999999987</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(B8-'2021-01-13'!$B8)</f>
+        <v>-0.60999999999999943</v>
+      </c>
+      <c r="H8" s="2">
+        <v>176213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>405.02</v>
+      </c>
+      <c r="C9" s="1">
+        <v>404.88</v>
+      </c>
+      <c r="D9" s="1">
+        <v>449</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13999999999998636</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>-43.980000000000018</v>
+      </c>
+      <c r="G9" s="6">
+        <f>(B9-'2021-01-13'!$B9)</f>
+        <v>-11.100000000000023</v>
+      </c>
+      <c r="H9" s="2">
+        <v>588141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>13.02</v>
+      </c>
+      <c r="D10" s="1">
+        <v>14.81</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7800000000000011</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.9999999999997868E-3</v>
+      </c>
+      <c r="G10" s="1">
+        <f>(B10-'2021-01-13'!$B10)</f>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6034</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7.09</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8.02</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.11000000000000032</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.8199999999999994</v>
+      </c>
+      <c r="G11" s="1">
+        <f>(B11-'2021-01-13'!$B11)</f>
+        <v>2.0000000000000462E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10848201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>82.02</v>
+      </c>
+      <c r="C12" s="1">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="D12" s="1">
+        <v>85.02</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.92000000000000171</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="G12" s="1">
+        <f>(B12-'2021-01-13'!$B12)</f>
+        <v>-0.32999999999999829</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6560059</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>213.22</v>
+      </c>
+      <c r="C13" s="1">
+        <v>212.09</v>
+      </c>
+      <c r="D13" s="1">
+        <v>220.41</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1299999999999955</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>-7.1899999999999977</v>
+      </c>
+      <c r="G13" s="6">
+        <f>(B13-'2021-01-13'!$B13)</f>
+        <v>-3.1200000000000045</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1776574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>129.74</v>
+      </c>
+      <c r="C14" s="1">
+        <v>109.18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>130.66999999999999</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>20.560000000000002</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.9299999999999784</v>
+      </c>
+      <c r="G14" s="3">
+        <f>(B14-'2021-01-13'!$B14)</f>
+        <v>5.6800000000000068</v>
+      </c>
+      <c r="H14" s="2">
+        <v>598974</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1">
+        <v>104.85</v>
+      </c>
+      <c r="C15" s="1">
+        <v>101.57</v>
+      </c>
+      <c r="D15" s="1">
+        <v>114.67</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>3.2800000000000011</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.8200000000000074</v>
+      </c>
+      <c r="G15" s="1">
+        <f>(B15-'2021-01-13'!$B15)</f>
+        <v>-2.2000000000000028</v>
+      </c>
+      <c r="H15" s="2">
+        <v>184096</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10.62</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9.77</v>
+      </c>
+      <c r="D16" s="1">
+        <v>10.86</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.84999999999999964</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.24000000000000021</v>
+      </c>
+      <c r="G16" s="1">
+        <f>(B16-'2021-01-13'!$B16)</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="H16" s="2">
+        <v>216926</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>40.25</v>
+      </c>
+      <c r="C17" s="1">
+        <v>36.81</v>
+      </c>
+      <c r="D17" s="1">
+        <v>41.72</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4399999999999977</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.4699999999999989</v>
+      </c>
+      <c r="G17" s="6">
+        <f>(B17-'2021-01-13'!$B17)</f>
+        <v>-1.1499999999999986</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1168304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>36.76</v>
+      </c>
+      <c r="C18" s="1">
+        <v>36.659999999999997</v>
+      </c>
+      <c r="D18" s="1">
+        <v>37.78</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.0200000000000031</v>
+      </c>
+      <c r="G18" s="1">
+        <f>(B18-'2021-01-13'!$B18)</f>
+        <v>-0.10999999999999943</v>
+      </c>
+      <c r="H18" s="2">
+        <v>21813953</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>70.95</v>
+      </c>
+      <c r="C19" s="1">
+        <v>68.709999999999994</v>
+      </c>
+      <c r="D19" s="1">
+        <v>72.349999999999994</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2400000000000091</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.3999999999999915</v>
+      </c>
+      <c r="G19" s="1">
+        <f>(B19-'2021-01-13'!$B19)</f>
+        <v>0.46999999999999886</v>
+      </c>
+      <c r="H19" s="2">
+        <v>5457302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1">
+        <v>124.71</v>
+      </c>
+      <c r="C20" s="1">
+        <v>124.04</v>
+      </c>
+      <c r="D20" s="1">
+        <v>135.35</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.66999999999998749</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>-10.64</v>
+      </c>
+      <c r="G20" s="1">
+        <f>(B20-'2021-01-13'!$B20)</f>
+        <v>-3.7900000000000063</v>
+      </c>
+      <c r="H20" s="2">
+        <v>375746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1">
+        <v>845</v>
+      </c>
+      <c r="C21" s="1">
+        <v>735.11</v>
+      </c>
+      <c r="D21" s="1">
+        <v>883.9</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>109.88999999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>-38.899999999999977</v>
+      </c>
+      <c r="G21" s="6">
+        <f>(B21-'2021-01-13'!$B21)</f>
+        <v>-9.4099999999999682</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1299348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>109.06</v>
+      </c>
+      <c r="C22" s="1">
+        <v>107.23</v>
+      </c>
+      <c r="D22" s="1">
+        <v>110.89</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8299999999999983</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.8299999999999983</v>
+      </c>
+      <c r="G22" s="1">
+        <f>(B22-'2021-01-13'!$B22)</f>
+        <v>0.15000000000000568</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1019192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1">
+        <v>226.12</v>
+      </c>
+      <c r="C23" s="1">
+        <v>223.04</v>
+      </c>
+      <c r="D23" s="1">
+        <v>237.66</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0800000000000125</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>-11.539999999999992</v>
+      </c>
+      <c r="G23" s="1">
+        <f>(B23-'2021-01-13'!$B23)</f>
+        <v>-0.97999999999998977</v>
+      </c>
+      <c r="H23" s="2">
+        <v>89954</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1">
+        <v>138.94</v>
+      </c>
+      <c r="C24" s="1">
+        <v>134.78</v>
+      </c>
+      <c r="D24" s="1">
+        <v>141.96</v>
+      </c>
+      <c r="E24" s="1">
+        <f>($B24-$C24)</f>
+        <v>4.1599999999999966</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.0200000000000102</v>
+      </c>
+      <c r="G24" s="3">
+        <f>(B24-'2021-01-13'!$B24)</f>
+        <v>2.5999999999999943</v>
+      </c>
+      <c r="H24" s="2">
+        <v>186505</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10.16</v>
+      </c>
+      <c r="C25" s="1">
+        <v>9.76</v>
+      </c>
+      <c r="D25" s="1">
+        <v>11.16</v>
+      </c>
+      <c r="E25" s="1">
+        <f>($B25-$C25)</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="F25" s="2">
+        <f>($B25-$D25)</f>
+        <v>-1</v>
+      </c>
+      <c r="G25" s="2">
+        <f>(B25-'2021-01-13'!$B25)</f>
+        <v>8.9999999999999858E-2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>20830</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1">
+        <v>72.459999999999994</v>
+      </c>
+      <c r="C26" s="1">
+        <v>65.709999999999994</v>
+      </c>
+      <c r="D26" s="1">
+        <v>72.459999999999994</v>
+      </c>
+      <c r="E26" s="2">
+        <f>($B26-$C26)</f>
+        <v>6.75</v>
+      </c>
+      <c r="F26" s="2">
+        <f>($B26-$D26)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <f>(B26-'2021-01-13'!$B26)</f>
+        <v>2.6799999999999926</v>
+      </c>
+      <c r="H26" s="2">
+        <v>373917</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1.6585000000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2.16</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27:E29" si="2">($B27-$C27)</f>
+        <v>0.43149999999999977</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" ref="F27:F29" si="3">($B27-$D27)</f>
+        <v>-7.0000000000000284E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <f>(B27-'2021-01-13'!$B27)</f>
+        <v>0.2699999999999998</v>
+      </c>
+      <c r="H27" s="2">
+        <v>316264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="1">
+        <v>126.07</v>
+      </c>
+      <c r="C28" s="1">
+        <v>125.9</v>
+      </c>
+      <c r="D28" s="1">
+        <v>129.29</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="2"/>
+        <v>0.16999999999998749</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.2199999999999989</v>
+      </c>
+      <c r="G28" s="2">
+        <f>(B28-'2021-01-13'!$B28)</f>
+        <v>-0.88000000000000966</v>
+      </c>
+      <c r="H28" s="2">
+        <v>575454</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1">
+        <v>34.76</v>
+      </c>
+      <c r="C29" s="1">
+        <v>32.83</v>
+      </c>
+      <c r="D29" s="1">
+        <v>35.06</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9299999999999997</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.30000000000000426</v>
+      </c>
+      <c r="G29" s="2">
+        <f>(B29-'2021-01-13'!$B29)</f>
+        <v>0.94999999999999574</v>
+      </c>
+      <c r="H29" s="2">
+        <v>42664076</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="1">
+        <v>49.23</v>
+      </c>
+      <c r="C30" s="1">
+        <v>49.23</v>
+      </c>
+      <c r="D30" s="1">
+        <v>50.51</v>
+      </c>
+      <c r="E30" s="2">
+        <f>($B30-$C30)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <f>($B30-$D30)</f>
+        <v>-1.2800000000000011</v>
+      </c>
+      <c r="G30" s="2">
+        <f>(B30-'2021-01-13'!$B30)</f>
+        <v>-0.92000000000000171</v>
+      </c>
+      <c r="H30" s="2">
+        <v>24548148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1">
+        <v>46.75</v>
+      </c>
+      <c r="C31" s="1">
+        <v>44.73</v>
+      </c>
+      <c r="D31" s="1">
+        <v>47.45</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" ref="E31" si="4">($B31-$C31)</f>
+        <v>2.0200000000000031</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31" si="5">($B31-$D31)</f>
+        <v>-0.70000000000000284</v>
+      </c>
+      <c r="G31" s="2">
+        <f>(B31-'2021-01-13'!$B31)</f>
+        <v>0.52000000000000313</v>
+      </c>
+      <c r="H31" s="2">
+        <v>54784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="1">
+        <v>209.91</v>
+      </c>
+      <c r="C32" s="1">
+        <v>205.47</v>
+      </c>
+      <c r="D32" s="1">
+        <v>214</v>
+      </c>
+      <c r="E32" s="2">
+        <f>($B32-$C32)</f>
+        <v>4.4399999999999977</v>
+      </c>
+      <c r="F32" s="2">
+        <f>($B32-$D32)</f>
+        <v>-4.0900000000000034</v>
+      </c>
+      <c r="G32" s="5">
+        <f>(B32-'2021-01-13'!$B32)</f>
+        <v>2.7199999999999989</v>
+      </c>
+      <c r="H32" s="2">
+        <v>10773046</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="1">
+        <v>143.69999999999999</v>
+      </c>
+      <c r="C33" s="1">
+        <v>142.15</v>
+      </c>
+      <c r="D33" s="1">
+        <v>147.91</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" ref="E33:E37" si="6">($B33-$C33)</f>
+        <v>1.5499999999999829</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" ref="F33:F37" si="7">($B33-$D33)</f>
+        <v>-4.210000000000008</v>
+      </c>
+      <c r="G33" s="2">
+        <f>(B33-'2021-01-13'!$B33)</f>
+        <v>0.46999999999999886</v>
+      </c>
+      <c r="H33" s="2">
+        <v>117744</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="1">
+        <v>69.03</v>
+      </c>
+      <c r="C34" s="1">
+        <v>66</v>
+      </c>
+      <c r="D34" s="1">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="6"/>
+        <v>3.0300000000000011</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="7"/>
+        <v>-0.37000000000000455</v>
+      </c>
+      <c r="G34" s="5">
+        <f>(B34-'2021-01-13'!$B34)</f>
+        <v>2.1599999999999966</v>
+      </c>
+      <c r="H34" s="2">
+        <v>22097754</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1.78</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="6"/>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="7"/>
+        <v>-0.11999999999999988</v>
+      </c>
+      <c r="G35" s="2">
+        <f>(B35-'2021-01-13'!$B35)</f>
+        <v>-2.0000000000000018E-2</v>
+      </c>
+      <c r="H35" s="2">
+        <v>219784</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1">
+        <v>27.05</v>
+      </c>
+      <c r="C36" s="1">
+        <v>26.48</v>
+      </c>
+      <c r="D36" s="1">
+        <v>27.58</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="6"/>
+        <v>0.57000000000000028</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="7"/>
+        <v>-0.52999999999999758</v>
+      </c>
+      <c r="G36" s="2">
+        <f>(B36-'2021-01-13'!$B36)</f>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1193495</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="1">
+        <v>146.93</v>
+      </c>
+      <c r="C37" s="1">
+        <v>146.07</v>
+      </c>
+      <c r="D37" s="1">
+        <v>148.44999999999999</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="6"/>
+        <v>0.86000000000001364</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="7"/>
+        <v>-1.5199999999999818</v>
+      </c>
+      <c r="G37" s="2">
+        <f>(B37-'2021-01-13'!$B37)</f>
+        <v>-0.54999999999998295</v>
+      </c>
+      <c r="H37" s="2">
+        <v>5432561</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="1">
+        <v>141.12</v>
+      </c>
+      <c r="C38" s="1">
+        <v>140.35</v>
+      </c>
+      <c r="D38" s="1">
+        <v>142.69</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" ref="E38:E41" si="8">($B38-$C38)</f>
+        <v>0.77000000000001023</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" ref="F38:F41" si="9">($B38-$D38)</f>
+        <v>-1.5699999999999932</v>
+      </c>
+      <c r="G38" s="2">
+        <f>(B38-'2021-01-13'!$B38)</f>
+        <v>141.12</v>
+      </c>
+      <c r="H38" s="2">
+        <v>13204891</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2.11</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="8"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="9"/>
+        <v>-2.0000000000000018E-2</v>
+      </c>
+      <c r="G39" s="2">
+        <f>(B39-'2021-01-13'!$B39)</f>
+        <v>2.09</v>
+      </c>
+      <c r="H39" s="2">
+        <v>3038333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="1">
+        <v>67.69</v>
+      </c>
+      <c r="C40" s="1">
+        <v>67.22</v>
+      </c>
+      <c r="D40" s="1">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.46999999999999886</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.74000000000000909</v>
+      </c>
+      <c r="G40" s="2">
+        <f>(B40-'2021-01-13'!$B40)</f>
+        <v>67.69</v>
+      </c>
+      <c r="H40" s="2">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="1">
+        <v>13.27</v>
+      </c>
+      <c r="C41" s="1">
+        <v>13.26</v>
+      </c>
+      <c r="D41" s="1">
+        <v>14.18</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="8"/>
+        <v>9.9999999999997868E-3</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="9"/>
+        <v>-0.91000000000000014</v>
+      </c>
+      <c r="G41" s="2">
+        <f>(B41-'2021-01-13'!$B41)</f>
+        <v>13.27</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1580154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>